<commit_message>
Few tests, halfway on the sponsored values refactoring.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0372639560d1acb6/Trabalho/Python/GitHub Desktop/Shopping_Auto_Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3939A33-8595-4001-898B-ABF548D1F30D}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A55ADDF-1A90-4218-9CF9-8A5BECA178EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
@@ -66,16 +66,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Bans</t>
-  </si>
-  <si>
-    <t>Forbidden Websites</t>
-  </si>
-  <si>
     <t>Min Value</t>
   </si>
   <si>
     <t>Max Value</t>
+  </si>
+  <si>
+    <t>Banned Words</t>
+  </si>
+  <si>
+    <t>Banned Websites</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,16 +460,16 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates on the product_search methods, fixing a few bugs
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0372639560d1acb6/Trabalho/Python/GitHub Desktop/Shopping_Auto_Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A55ADDF-1A90-4218-9CF9-8A5BECA178EF}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{4B42EEB8-E014-4F6F-8E3A-37E95301BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF83FAC9-E6C6-4DCB-9893-1231C5C19D08}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD3F9E8B-8E7C-43BA-8194-A874F6873E6D}"/>
   </bookViews>
@@ -34,28 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>iphone 14 pro max 128 gb</t>
-  </si>
-  <si>
-    <t>rtx 4060 ti</t>
-  </si>
-  <si>
-    <t>3060 3070 4070 3080</t>
-  </si>
-  <si>
-    <t>macbook 16 gb</t>
-  </si>
-  <si>
-    <t>aliexpress tiendamia shopee enjoei locadora tudoiphone</t>
-  </si>
-  <si>
-    <t>mini watch 11 13 usado</t>
-  </si>
-  <si>
-    <t>patoloco aliexpress</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>horizonplay goimports conceitoapple lojamsimportados voltsdistribuidor e-dealstore iphonevendasx bludiode tradeinn</t>
   </si>
@@ -76,13 +55,46 @@
   </si>
   <si>
     <t>Banned Websites</t>
+  </si>
+  <si>
+    <t>rtx 4060 ti 16 gb</t>
+  </si>
+  <si>
+    <t>3060 3070 4070 3080 8</t>
+  </si>
+  <si>
+    <t>ryzen 5800x3d</t>
+  </si>
+  <si>
+    <t>logitech g733</t>
+  </si>
+  <si>
+    <t>iphone 15 pro max 256 gb</t>
+  </si>
+  <si>
+    <t>mini watch 11 12 13 14 usado</t>
+  </si>
+  <si>
+    <t>macbook 16 gb m2</t>
+  </si>
+  <si>
+    <t>5700x</t>
+  </si>
+  <si>
+    <t>g535</t>
+  </si>
+  <si>
+    <t>patoloco aliexpress techinn shopee</t>
+  </si>
+  <si>
+    <t>aliexpress tiendamia shopee enjoei ebay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +104,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,87 +461,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220DEAF8-BE44-4105-B361-44B3C8893CB3}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
+    <col min="3" max="3" width="110" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2">
-        <v>5500</v>
+        <v>8000</v>
       </c>
       <c r="E2">
-        <v>9000</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="E3">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>5000</v>
-      </c>
-      <c r="E4">
+        <v>5500</v>
+      </c>
+      <c r="E4" s="2">
         <v>11000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1500</v>
+      </c>
+      <c r="E5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2">
+        <v>600</v>
+      </c>
+      <c r="E6" s="2">
+        <v>920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>